<commit_message>
motors, pumps and valves selected
</commit_message>
<xml_diff>
--- a/akční členy.xlsx
+++ b/akční členy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radim\Desktop\git\project_AUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3102320-0F83-4441-897F-688D3D8F2ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDC5D88-C6D3-47FF-84F2-8A6418B09314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>označení</t>
   </si>
@@ -39,12 +39,6 @@
     <t>V01.03</t>
   </si>
   <si>
-    <t>A01.01</t>
-  </si>
-  <si>
-    <t>pasterizační tank</t>
-  </si>
-  <si>
     <t>M01.01</t>
   </si>
   <si>
@@ -145,24 +139,6 @@
   </si>
   <si>
     <t>napouštěcí ventil nádrže s čistou vodou</t>
-  </si>
-  <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>nádrž s čistou vodou</t>
-  </si>
-  <si>
-    <t>nádrž s použitou vodou</t>
-  </si>
-  <si>
-    <t>nádrž s louhem</t>
   </si>
   <si>
     <t>vstupní ventil čisté vody</t>
@@ -555,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C29"/>
+  <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -580,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -588,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -596,15 +572,15 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -612,84 +588,84 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
@@ -697,98 +673,66 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>45</v>
+      <c r="C25" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>